<commit_message>
Deploying to gh-pages from  @ 09d067ec778cd095c100d07675da68c28286de85 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/15.2.1.xlsx
+++ b/en/downloads/data-excel/15.2.1.xlsx
@@ -559,11 +559,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -575,7 +573,7 @@
     <col min="6" max="8" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -592,7 +590,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
       <c r="C2" s="8"/>
@@ -603,7 +601,7 @@
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
     </row>
-    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
@@ -643,8 +641,11 @@
       <c r="M3" s="12">
         <v>2022</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N3" s="12">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>10</v>
       </c>
@@ -682,10 +683,13 @@
         <v>212.1</v>
       </c>
       <c r="M4" s="14">
-        <v>723.8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="24" x14ac:dyDescent="0.25">
+        <v>923.8</v>
+      </c>
+      <c r="N4" s="14">
+        <v>583.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>11</v>
       </c>
@@ -723,8 +727,9 @@
         <v>18</v>
       </c>
       <c r="M5" s="17"/>
-    </row>
-    <row r="6" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N5" s="17"/>
+    </row>
+    <row r="6" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>12</v>
       </c>
@@ -762,8 +767,9 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="M6" s="14"/>
-    </row>
-    <row r="7" spans="1:13" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N6" s="14"/>
+    </row>
+    <row r="7" spans="1:14" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>13</v>
       </c>
@@ -801,10 +807,13 @@
         <v>64</v>
       </c>
       <c r="M7" s="16">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+        <v>64.03</v>
+      </c>
+      <c r="N7" s="16">
+        <v>64.08</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -815,7 +824,7 @@
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -826,7 +835,7 @@
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -837,7 +846,7 @@
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -848,7 +857,7 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -859,7 +868,7 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>

</xml_diff>